<commit_message>
Advance integration of MESSAGE. Fix LCIs for electrolyzers. Fix translation of outdated biosphere flows. Update docs.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-synfuels-from-FT-from-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-synfuels-from-FT-from-electrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CB21D4-A44E-CF48-A451-B243E8E6BDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B5020E-0498-2645-8BDE-20400E53D9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="1960" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FT Process description" sheetId="2" r:id="rId1"/>
@@ -496,10 +496,10 @@
     <t>ecoinvent</t>
   </si>
   <si>
-    <t>hydrogen production, gaseous, 200 bar, from PEM electrolysis, from grid electricity</t>
-  </si>
-  <si>
-    <t>hydrogen, gaseous, 200 bar</t>
+    <t>hydrogen production, gaseous, 30 bar, from PEM electrolysis, from grid electricity</t>
+  </si>
+  <si>
+    <t>hydrogen, gaseous, 30 bar</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1570,7 @@
   <dimension ref="A1:K638"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G639" sqref="G639"/>
+      <selection activeCell="K654" sqref="K654"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6466,7 +6466,7 @@
   <autoFilter ref="A1:K638" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="hydrogen production, gaseous, 25 bar, from electrolysis"/>
+        <filter val="hydrogen production, gaseous, 200 bar, from PEM electrolysis, from grid electricity"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>